<commit_message>
Updates internal schema + Adds a search box for action
</commit_message>
<xml_diff>
--- a/solutions/SiteDesignsStudio/dev_assets/schema_loc_resources.xlsx
+++ b/solutions/SiteDesignsStudio/dev_assets/schema_loc_resources.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\labs\ypcode\spfx-site-designs-studio\dev_assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\repo\ypcode\sp-dev-solutions\solutions\SiteDesignsStudio\dev_assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DDDF03EF-9A67-45F1-9CF1-39C7978D0FFD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E829CD7A-974D-486F-8A14-5351793761F3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9615" activeTab="1" xr2:uid="{D882761B-9DBF-4D1F-9EAC-403D9E335D43}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9615" xr2:uid="{D882761B-9DBF-4D1F-9EAC-403D9E335D43}"/>
   </bookViews>
   <sheets>
     <sheet name="Actions en-US" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="148">
   <si>
     <t>Title</t>
   </si>
@@ -362,6 +362,114 @@
   </si>
   <si>
     <t>The defined external sharing capability</t>
+  </si>
+  <si>
+    <t>enforceUnique</t>
+  </si>
+  <si>
+    <t>Enforce Unique value</t>
+  </si>
+  <si>
+    <t>createSPList_addSPFieldXml</t>
+  </si>
+  <si>
+    <t>Add a field as XML</t>
+  </si>
+  <si>
+    <t>Add a field to the list using its XML schema</t>
+  </si>
+  <si>
+    <t>schemaXml</t>
+  </si>
+  <si>
+    <t>Field XML Schema</t>
+  </si>
+  <si>
+    <t>The XML Schema of the field to add</t>
+  </si>
+  <si>
+    <t>(Optional) Specifies wheter all values for this field must be unique</t>
+  </si>
+  <si>
+    <t>internalName</t>
+  </si>
+  <si>
+    <t>Internal Name</t>
+  </si>
+  <si>
+    <t>(Optional) The internal name of the field</t>
+  </si>
+  <si>
+    <t>createSPList_addSPView</t>
+  </si>
+  <si>
+    <t>Add a view</t>
+  </si>
+  <si>
+    <t>Defines and adds a view to the list</t>
+  </si>
+  <si>
+    <t>createSPList_removeSPView</t>
+  </si>
+  <si>
+    <t>Remove a view</t>
+  </si>
+  <si>
+    <t>Remove a view from the list</t>
+  </si>
+  <si>
+    <t>createContentType_addSiteColumn</t>
+  </si>
+  <si>
+    <t>Add a site column</t>
+  </si>
+  <si>
+    <t>Add a site column to the Content Type</t>
+  </si>
+  <si>
+    <t>createContentType_removeSiteColumn</t>
+  </si>
+  <si>
+    <t>Remove a site column</t>
+  </si>
+  <si>
+    <t>Remove a column from the Content Type</t>
+  </si>
+  <si>
+    <t>createSiteColumn</t>
+  </si>
+  <si>
+    <t>Create Site Column</t>
+  </si>
+  <si>
+    <t>Create a new Site Column</t>
+  </si>
+  <si>
+    <t>createContentType</t>
+  </si>
+  <si>
+    <t>Create Site Content Type</t>
+  </si>
+  <si>
+    <t>Create a new Site Content Type</t>
+  </si>
+  <si>
+    <t>installSPFXSolution</t>
+  </si>
+  <si>
+    <t>Install a SPFx Solution or Addin</t>
+  </si>
+  <si>
+    <t>Install a SharePoint Framework solution (or add-in) to the site</t>
+  </si>
+  <si>
+    <t>setRegionalSettings</t>
+  </si>
+  <si>
+    <t>Set regional settings</t>
+  </si>
+  <si>
+    <t>Set the regional settings of the site</t>
   </si>
 </sst>
 </file>
@@ -427,15 +535,15 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -470,8 +578,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D41D1B67-316F-44FF-89F7-18228FD63C60}" name="Table1" displayName="Table1" ref="A1:G15" totalsRowShown="0">
-  <autoFilter ref="A1:G15" xr:uid="{63EE1810-E1DD-440A-BD6A-89F18F476329}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D41D1B67-316F-44FF-89F7-18228FD63C60}" name="Table1" displayName="Table1" ref="A1:G24" totalsRowShown="0">
+  <autoFilter ref="A1:G24" xr:uid="{63EE1810-E1DD-440A-BD6A-89F18F476329}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{0CA43AC1-7A38-4572-A307-3B9C459DA269}" name="Id"/>
     <tableColumn id="2" xr3:uid="{43B8C421-D995-417E-97CD-F5AF9CCE1833}" name="Title"/>
@@ -488,8 +596,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A0DDDC5B-90A9-4FD9-960B-532152CF3A2D}" name="Table13" displayName="Table13" ref="A1:H25" totalsRowShown="0">
-  <autoFilter ref="A1:H25" xr:uid="{5B74A50E-37C8-450E-9F21-0943BD6E8407}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A0DDDC5B-90A9-4FD9-960B-532152CF3A2D}" name="Table13" displayName="Table13" ref="A1:H29" totalsRowShown="0">
+  <autoFilter ref="A1:H29" xr:uid="{5B74A50E-37C8-450E-9F21-0943BD6E8407}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{8133C111-3D12-498B-96AE-A1B87FC3E5FE}" name="Action"/>
     <tableColumn id="8" xr3:uid="{A955F4A9-AF04-4D90-A3A6-1B27E4867332}" name="Property"/>
@@ -497,11 +605,11 @@
     <tableColumn id="3" xr3:uid="{4B0813AC-12FA-4544-B1FA-17A20BD3222B}" name="Title Resource Key" dataDxfId="3">
       <calculatedColumnFormula>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{9A6F0D91-3E33-4A2F-BF91-979D3F80A3E0}" name="Title Resource" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{9A6F0D91-3E33-4A2F-BF91-979D3F80A3E0}" name="Title Resource" dataDxfId="2">
       <calculatedColumnFormula>D2&amp;":"""&amp;C2&amp;""","</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{0DB5ED8E-BCAA-45A9-9625-2B1E8354D28D}" name="Description"/>
-    <tableColumn id="6" xr3:uid="{246A9136-D3AD-447A-893C-776E69CD6EA5}" name="Description Resource Key" dataDxfId="2">
+    <tableColumn id="6" xr3:uid="{246A9136-D3AD-447A-893C-776E69CD6EA5}" name="Description Resource Key" dataDxfId="1">
       <calculatedColumnFormula>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{06231D2F-2C63-428B-B50E-22B122D96768}" name="Description Resource" dataDxfId="0">
@@ -809,21 +917,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED73395-32B4-450D-90B8-56CF29C8764F}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="34.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.1328125" customWidth="1"/>
-    <col min="6" max="6" width="45.53125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="97.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.9296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.73046875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="46.265625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="43.46484375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.53125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="97.46484375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
@@ -884,22 +992,22 @@
         <v>23</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C15" si="0">SUBSTITUTE("Schema_Action_${value}_Title","${value}",A3)</f>
+        <f t="shared" ref="C3:C20" si="0">SUBSTITUTE("Schema_Action_${value}_Title","${value}",A3)</f>
         <v>Schema_Action_createSPList_setDescription_Title</v>
       </c>
       <c r="D3" s="1" t="str">
-        <f t="shared" ref="D3:D15" si="1">C3&amp;":'"&amp;B3&amp;"',"</f>
+        <f t="shared" ref="D3:D20" si="1">C3&amp;":'"&amp;B3&amp;"',"</f>
         <v>Schema_Action_createSPList_setDescription_Title:'Set the description',</v>
       </c>
       <c r="E3" t="s">
         <v>25</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F13" si="2">SUBSTITUTE("Schema_Action_createSPList_${value}_Desc","${value}",A3)</f>
+        <f t="shared" ref="F3:F20" si="2">SUBSTITUTE("Schema_Action_createSPList_${value}_Desc","${value}",A3)</f>
         <v>Schema_Action_createSPList_createSPList_setDescription_Desc</v>
       </c>
       <c r="G3" s="1" t="str">
-        <f t="shared" ref="G3:G13" si="3">F3&amp;":'"&amp;E3&amp;"',"</f>
+        <f t="shared" ref="G3:G20" si="3">F3&amp;":'"&amp;E3&amp;"',"</f>
         <v>Schema_Action_createSPList_createSPList_setDescription_Desc:'Set the description of the list',</v>
       </c>
     </row>
@@ -959,271 +1067,426 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>Schema_Action_createSPList_addSPFieldXml_Title</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Schema_Action_createSPList_addSPFieldXml_Title:'Add a field as XML',</v>
+      </c>
+      <c r="E6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" ref="F6" si="4">SUBSTITUTE("Schema_Action_createSPList_${value}_Desc","${value}",A6)</f>
+        <v>Schema_Action_createSPList_createSPList_addSPFieldXml_Desc</v>
+      </c>
+      <c r="G6" s="1" t="str">
+        <f t="shared" ref="G6" si="5">F6&amp;":'"&amp;E6&amp;"',"</f>
+        <v>Schema_Action_createSPList_createSPList_addSPFieldXml_Desc:'Add a field to the list using its XML schema',</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G7" s="1" t="str">
+        <f>F7&amp;":'"&amp;E7&amp;"',"</f>
+        <v>:'Defines and adds a view to the list',</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" t="s">
+        <v>129</v>
+      </c>
+      <c r="G8" s="1" t="str">
+        <f>F8&amp;":'"&amp;E8&amp;"',"</f>
+        <v>:'Remove a view from the list',</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C6" t="str">
+      <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>Schema_Action_createSPList_addContentType_Title</v>
       </c>
-      <c r="D6" s="1" t="str">
+      <c r="D9" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Schema_Action_createSPList_addContentType_Title:'Add a Content Type',</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E9" t="s">
         <v>33</v>
       </c>
-      <c r="F6" t="str">
+      <c r="F9" t="str">
         <f t="shared" si="2"/>
         <v>Schema_Action_createSPList_createSPList_addContentType_Desc</v>
       </c>
-      <c r="G6" s="1" t="str">
+      <c r="G9" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Schema_Action_createSPList_createSPList_addContentType_Desc:'Add one of the available Site Content Types to the list',</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C7" t="str">
+      <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>Schema_Action_createSPList_removeContentType_Title</v>
       </c>
-      <c r="D7" s="1" t="str">
+      <c r="D10" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Schema_Action_createSPList_removeContentType_Title:'Remove a Content Type',</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E10" t="s">
         <v>34</v>
       </c>
-      <c r="F7" t="str">
+      <c r="F10" t="str">
         <f t="shared" si="2"/>
         <v>Schema_Action_createSPList_createSPList_removeContentType_Desc</v>
       </c>
-      <c r="G7" s="1" t="str">
+      <c r="G10" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Schema_Action_createSPList_createSPList_removeContentType_Desc:'Remove a Content Type from the list',</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B11" t="s">
         <v>35</v>
       </c>
-      <c r="C8" t="str">
+      <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>Schema_Action_createSPList_setSPFieldCustomFormatter_Title</v>
       </c>
-      <c r="D8" s="1" t="str">
+      <c r="D11" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Schema_Action_createSPList_setSPFieldCustomFormatter_Title:'Set a field custom formatter',</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E11" t="s">
         <v>36</v>
       </c>
-      <c r="F8" t="str">
+      <c r="F11" t="str">
         <f t="shared" si="2"/>
         <v>Schema_Action_createSPList_createSPList_setSPFieldCustomFormatter_Desc</v>
       </c>
-      <c r="G8" s="1" t="str">
+      <c r="G11" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Schema_Action_createSPList_createSPList_setSPFieldCustomFormatter_Desc:'Set a custom formatter for a specific field',</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" t="s">
+        <v>132</v>
+      </c>
+      <c r="G12" s="1" t="str">
+        <f>F12&amp;":'"&amp;E12&amp;"',"</f>
+        <v>:'Add a site column to the Content Type',</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" t="s">
+        <v>135</v>
+      </c>
+      <c r="G13" s="1" t="str">
+        <f>F13&amp;":'"&amp;E13&amp;"',"</f>
+        <v>:'Remove a column from the Content Type',</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" t="s">
+        <v>138</v>
+      </c>
+      <c r="G14" s="1" t="str">
+        <f>F14&amp;":'"&amp;E14&amp;"',"</f>
+        <v>:'Create a new Site Column',</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B15" t="s">
+        <v>140</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" t="s">
+        <v>141</v>
+      </c>
+      <c r="G15" s="1" t="str">
+        <f>F15&amp;":'"&amp;E15&amp;"',"</f>
+        <v>:'Create a new Site Content Type',</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B16" t="s">
         <v>37</v>
       </c>
-      <c r="C9" t="str">
+      <c r="C16" t="str">
         <f t="shared" si="0"/>
         <v>Schema_Action_createSPList_Title</v>
       </c>
-      <c r="D9" s="1" t="str">
+      <c r="D16" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Schema_Action_createSPList_Title:'Create a List',</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E16" t="s">
         <v>42</v>
       </c>
-      <c r="F9" t="str">
+      <c r="F16" t="str">
         <f t="shared" si="2"/>
         <v>Schema_Action_createSPList_createSPList_Desc</v>
       </c>
-      <c r="G9" s="1" t="str">
+      <c r="G16" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Schema_Action_createSPList_createSPList_Desc:'Create in list in the current site',</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B17" t="s">
         <v>38</v>
       </c>
-      <c r="C10" t="str">
+      <c r="C17" t="str">
         <f t="shared" si="0"/>
         <v>Schema_Action_addNavLink_Title</v>
       </c>
-      <c r="D10" s="1" t="str">
+      <c r="D17" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Schema_Action_addNavLink_Title:'Add a navigation link',</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E17" t="s">
         <v>43</v>
       </c>
-      <c r="F10" t="str">
+      <c r="F17" t="str">
         <f t="shared" si="2"/>
         <v>Schema_Action_createSPList_addNavLink_Desc</v>
       </c>
-      <c r="G10" s="1" t="str">
+      <c r="G17" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Schema_Action_createSPList_addNavLink_Desc:'Add a Navigation Link to the current site',</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B18" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="str">
+      <c r="C18" t="str">
         <f t="shared" si="0"/>
         <v>Schema_Action_applyTheme_Title</v>
       </c>
-      <c r="D11" s="1" t="str">
+      <c r="D18" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Schema_Action_applyTheme_Title:'Apply a theme',</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E18" t="s">
         <v>44</v>
       </c>
-      <c r="F11" t="str">
+      <c r="F18" t="str">
         <f t="shared" si="2"/>
         <v>Schema_Action_createSPList_applyTheme_Desc</v>
       </c>
-      <c r="G11" s="1" t="str">
+      <c r="G18" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Schema_Action_createSPList_applyTheme_Desc:'Apply a custom theme to the current site',</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B19" t="s">
         <v>39</v>
       </c>
-      <c r="C12" t="str">
+      <c r="C19" t="str">
         <f t="shared" si="0"/>
         <v>Schema_Action_setSiteLogo_Title</v>
       </c>
-      <c r="D12" s="1" t="str">
+      <c r="D19" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Schema_Action_setSiteLogo_Title:'Set the Site Logo',</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E19" t="s">
         <v>45</v>
       </c>
-      <c r="F12" t="str">
+      <c r="F19" t="str">
         <f t="shared" si="2"/>
         <v>Schema_Action_createSPList_setSiteLogo_Desc</v>
       </c>
-      <c r="G12" s="1" t="str">
+      <c r="G19" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Schema_Action_createSPList_setSiteLogo_Desc:'Set the logo of the current site',</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B20" t="s">
         <v>40</v>
       </c>
-      <c r="C13" t="str">
+      <c r="C20" t="str">
         <f t="shared" si="0"/>
         <v>Schema_Action_joinHubSite_Title</v>
       </c>
-      <c r="D13" s="1" t="str">
+      <c r="D20" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Schema_Action_joinHubSite_Title:'Join a Hub Site',</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E20" t="s">
         <v>46</v>
       </c>
-      <c r="F13" t="str">
+      <c r="F20" t="str">
         <f t="shared" si="2"/>
         <v>Schema_Action_createSPList_joinHubSite_Desc</v>
       </c>
-      <c r="G13" s="1" t="str">
+      <c r="G20" s="1" t="str">
         <f t="shared" si="3"/>
         <v>Schema_Action_createSPList_joinHubSite_Desc:'Make the current site join a specified Hub Site',</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>142</v>
+      </c>
+      <c r="B21" t="s">
+        <v>143</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" t="s">
+        <v>144</v>
+      </c>
+      <c r="G21" s="1" t="str">
+        <f>F21&amp;":'"&amp;E21&amp;"',"</f>
+        <v>:'Install a SharePoint Framework solution (or add-in) to the site',</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B22" t="s">
         <v>41</v>
       </c>
-      <c r="C14" t="str">
-        <f>SUBSTITUTE("Schema_Action_${value}_Title","${value}",A14)</f>
+      <c r="C22" t="str">
+        <f>SUBSTITUTE("Schema_Action_${value}_Title","${value}",A22)</f>
         <v>Schema_Action_triggerFlow_Title</v>
       </c>
-      <c r="D14" s="1" t="str">
-        <f>C14&amp;":'"&amp;B14&amp;"',"</f>
+      <c r="D22" s="1" t="str">
+        <f>C22&amp;":'"&amp;B22&amp;"',"</f>
         <v>Schema_Action_triggerFlow_Title:'Trigger a Flow',</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E22" t="s">
         <v>47</v>
       </c>
-      <c r="F14" t="str">
-        <f>SUBSTITUTE("Schema_Action_createSPList_${value}_Desc","${value}",A14)</f>
+      <c r="F22" t="str">
+        <f>SUBSTITUTE("Schema_Action_createSPList_${value}_Desc","${value}",A22)</f>
         <v>Schema_Action_createSPList_triggerFlow_Desc</v>
       </c>
-      <c r="G14" s="1" t="str">
-        <f>F14&amp;":'"&amp;E14&amp;"',"</f>
+      <c r="G22" s="1" t="str">
+        <f>F22&amp;":'"&amp;E22&amp;"',"</f>
         <v>Schema_Action_createSPList_triggerFlow_Desc:'Trigger the specified Microsoft Flow',</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>145</v>
+      </c>
+      <c r="B23" t="s">
+        <v>146</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" t="s">
+        <v>147</v>
+      </c>
+      <c r="G23" s="1" t="str">
+        <f>F23&amp;":'"&amp;E23&amp;"',"</f>
+        <v>:'Set the regional settings of the site',</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
         <v>106</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B24" t="s">
         <v>107</v>
       </c>
-      <c r="C15" t="str">
-        <f>SUBSTITUTE("Schema_Action_${value}_Title","${value}",A15)</f>
+      <c r="C24" t="str">
+        <f>SUBSTITUTE("Schema_Action_${value}_Title","${value}",A24)</f>
         <v>Schema_Action_setSiteExternalSharingCapability_Title</v>
       </c>
-      <c r="D15" s="1" t="str">
-        <f>C15&amp;":'"&amp;B15&amp;"',"</f>
+      <c r="D24" s="1" t="str">
+        <f>C24&amp;":'"&amp;B24&amp;"',"</f>
         <v>Schema_Action_setSiteExternalSharingCapability_Title:'Set site external sharing capability',</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E24" t="s">
         <v>108</v>
       </c>
-      <c r="F15" t="str">
-        <f>SUBSTITUTE("Schema_Action_createSPList_${value}_Desc","${value}",A15)</f>
+      <c r="F24" t="str">
+        <f>SUBSTITUTE("Schema_Action_createSPList_${value}_Desc","${value}",A24)</f>
         <v>Schema_Action_createSPList_setSiteExternalSharingCapability_Desc</v>
       </c>
-      <c r="G15" s="1" t="str">
-        <f>F15&amp;":'"&amp;E15&amp;"',"</f>
+      <c r="G24" s="1" t="str">
+        <f>F24&amp;":'"&amp;E24&amp;"',"</f>
         <v>Schema_Action_createSPList_setSiteExternalSharingCapability_Desc:'Set the external sharing capability of the site',</v>
       </c>
     </row>
@@ -1238,10 +1501,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A573984-D07C-4EF1-8ACE-63C3D1838851}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1249,11 +1512,11 @@
     <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.33203125" customWidth="1"/>
     <col min="3" max="3" width="23.06640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="75.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="75.33203125" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="43.46484375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="61.796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="97.46484375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61.796875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="97.46484375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
@@ -1297,7 +1560,7 @@
         <v>Schema_createSPList_setTitle_title_Title</v>
       </c>
       <c r="E2" s="1" t="str">
-        <f t="shared" ref="E2:E25" si="0">D2&amp;":"""&amp;C2&amp;""","</f>
+        <f t="shared" ref="E2:E29" si="0">D2&amp;":"""&amp;C2&amp;""","</f>
         <v>Schema_createSPList_setTitle_title_Title:"Title",</v>
       </c>
       <c r="F2" t="s">
@@ -1308,7 +1571,7 @@
         <v>Schema_createSPList_setTitle_title_Desc</v>
       </c>
       <c r="H2" s="1" t="str">
-        <f t="shared" ref="H2:H25" si="1">G2&amp;":"""&amp;F2&amp;""","</f>
+        <f t="shared" ref="H2:H29" si="1">G2&amp;":"""&amp;F2&amp;""","</f>
         <v>Schema_createSPList_setTitle_title_Desc:"Title of the list",</v>
       </c>
     </row>
@@ -1402,602 +1665,722 @@
         <v>Schema_createSPList_addSPField_displayName_Desc:"The displayed name of the field",</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="4" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_createSPList_addSPField_isRequired_Title</v>
-      </c>
-      <c r="E6" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Schema_createSPList_addSPField_isRequired_Title:"Is required",</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G6" s="4" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_createSPList_addSPField_isRequired_Desc</v>
-      </c>
-      <c r="H6" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Schema_createSPList_addSPField_isRequired_Desc:"Is the field required",</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="2" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_createSPList_addSPField_internalName_Title</v>
+      </c>
+      <c r="E6" s="6" t="str">
+        <f>D6&amp;":"""&amp;C6&amp;""","</f>
+        <v>Schema_createSPList_addSPField_internalName_Title:"Internal Name",</v>
+      </c>
+      <c r="F6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" s="2" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_createSPList_addSPField_internalName_Desc</v>
+      </c>
+      <c r="H6" s="6" t="str">
+        <f>G6&amp;":"""&amp;F6&amp;""","</f>
+        <v>Schema_createSPList_addSPField_internalName_Desc:"(Optional) The internal name of the field",</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="2" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_createSPList_addSPField_addToDefaultView_Title</v>
-      </c>
-      <c r="E7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Schema_createSPList_addSPField_addToDefaultView_Title:"Add to default view",</v>
-      </c>
-      <c r="F7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G7" s="2" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_createSPList_addSPField_addToDefaultView_Desc</v>
-      </c>
-      <c r="H7" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Schema_createSPList_addSPField_addToDefaultView_Desc:"The field is added to default view",</v>
+      <c r="B7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="4" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_createSPList_addSPField_isRequired_Title</v>
+      </c>
+      <c r="E7" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Schema_createSPList_addSPField_isRequired_Title:"Is required",</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="4" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_createSPList_addSPField_isRequired_Desc</v>
+      </c>
+      <c r="H7" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>Schema_createSPList_addSPField_isRequired_Desc:"Is the field required",</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D8" s="2" t="str">
         <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_createSPList_deleteSPField_displayName_Title</v>
+        <v>Schema_createSPList_addSPField_addToDefaultView_Title</v>
       </c>
       <c r="E8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Schema_createSPList_deleteSPField_displayName_Title:"Display Name",</v>
+        <v>Schema_createSPList_addSPField_addToDefaultView_Title:"Add to default view",</v>
       </c>
       <c r="F8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G8" s="2" t="str">
         <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_createSPList_deleteSPField_displayName_Desc</v>
+        <v>Schema_createSPList_addSPField_addToDefaultView_Desc</v>
       </c>
       <c r="H8" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Schema_createSPList_deleteSPField_displayName_Desc:"The displayed name of the field",</v>
+        <v>Schema_createSPList_addSPField_addToDefaultView_Desc:"The field is added to default view",</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>112</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="D9" s="2" t="str">
         <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_createSPList_addContentType_name_Title</v>
-      </c>
-      <c r="E9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Schema_createSPList_addContentType_name_Title:"Content Type's name",</v>
+        <v>Schema_createSPList_addSPField_enforceUnique_Title</v>
+      </c>
+      <c r="E9" s="6" t="str">
+        <f>D9&amp;":"""&amp;C9&amp;""","</f>
+        <v>Schema_createSPList_addSPField_enforceUnique_Title:"Enforce Unique value",</v>
       </c>
       <c r="F9" t="s">
-        <v>66</v>
+        <v>120</v>
       </c>
       <c r="G9" s="2" t="str">
         <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_createSPList_addContentType_name_Desc</v>
-      </c>
-      <c r="H9" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Schema_createSPList_addContentType_name_Desc:"The name of an existing Site Content Type",</v>
+        <v>Schema_createSPList_addSPField_enforceUnique_Desc</v>
+      </c>
+      <c r="H9" s="6" t="str">
+        <f>G9&amp;":"""&amp;F9&amp;""","</f>
+        <v>Schema_createSPList_addSPField_enforceUnique_Desc:"(Optional) Specifies wheter all values for this field must be unique",</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D10" s="2" t="str">
         <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_createSPList_removeContentType_name_Title</v>
+        <v>Schema_createSPList_deleteSPField_displayName_Title</v>
       </c>
       <c r="E10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Schema_createSPList_removeContentType_name_Title:"Content Type's name",</v>
+        <v>Schema_createSPList_deleteSPField_displayName_Title:"Display Name",</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G10" s="2" t="str">
         <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_createSPList_removeContentType_name_Desc</v>
+        <v>Schema_createSPList_deleteSPField_displayName_Desc</v>
       </c>
       <c r="H10" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Schema_createSPList_removeContentType_name_Desc:"The name of the Content Type",</v>
+        <v>Schema_createSPList_deleteSPField_displayName_Desc:"The displayed name of the field",</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>117</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_createSPList_setSPFieldCustomFormatter_fieldDisplayName_Title</v>
-      </c>
-      <c r="E11" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Schema_createSPList_setSPFieldCustomFormatter_fieldDisplayName_Title:"Field's display name",</v>
+        <v>118</v>
+      </c>
+      <c r="D11" s="2" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_createSPList_addSPFieldXml_schemaXml_Title</v>
+      </c>
+      <c r="E11" s="6" t="str">
+        <f>D11&amp;":"""&amp;C11&amp;""","</f>
+        <v>Schema_createSPList_addSPFieldXml_schemaXml_Title:"Field XML Schema",</v>
       </c>
       <c r="F11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G11" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_createSPList_setSPFieldCustomFormatter_fieldDisplayName_Desc</v>
-      </c>
-      <c r="H11" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Schema_createSPList_setSPFieldCustomFormatter_fieldDisplayName_Desc:"The display name of the field to apply the formatting on",</v>
+        <v>119</v>
+      </c>
+      <c r="G11" s="2" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_createSPList_addSPFieldXml_schemaXml_Desc</v>
+      </c>
+      <c r="H11" s="6" t="str">
+        <f>G11&amp;":"""&amp;F11&amp;""","</f>
+        <v>Schema_createSPList_addSPFieldXml_schemaXml_Desc:"The XML Schema of the field to add",</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_createSPList_setSPFieldCustomFormatter_formatterJSON_Title</v>
-      </c>
-      <c r="E12" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Schema_createSPList_setSPFieldCustomFormatter_formatterJSON_Title:"The formatter JSON",</v>
+        <v>59</v>
+      </c>
+      <c r="D12" s="2" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_createSPList_addSPFieldXml_addToDefaultView_Title</v>
+      </c>
+      <c r="E12" s="6" t="str">
+        <f>D12&amp;":"""&amp;C12&amp;""","</f>
+        <v>Schema_createSPList_addSPFieldXml_addToDefaultView_Title:"Add to default view",</v>
       </c>
       <c r="F12" t="s">
-        <v>73</v>
-      </c>
-      <c r="G12" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_createSPList_setSPFieldCustomFormatter_formatterJSON_Desc</v>
-      </c>
-      <c r="H12" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Schema_createSPList_setSPFieldCustomFormatter_formatterJSON_Desc:"The formatter rules expressed in JSON",</v>
+        <v>60</v>
+      </c>
+      <c r="G12" s="2" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_createSPList_addSPFieldXml_addToDefaultView_Desc</v>
+      </c>
+      <c r="H12" s="6" t="str">
+        <f>G12&amp;":"""&amp;F12&amp;""","</f>
+        <v>Schema_createSPList_addSPFieldXml_addToDefaultView_Desc:"The field is added to default view",</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_createSPList_listName_Title</v>
+        <v>65</v>
+      </c>
+      <c r="D13" s="2" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_createSPList_addContentType_name_Title</v>
       </c>
       <c r="E13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Schema_createSPList_listName_Title:"List's name",</v>
+        <v>Schema_createSPList_addContentType_name_Title:"Content Type's name",</v>
       </c>
       <c r="F13" t="s">
-        <v>80</v>
-      </c>
-      <c r="G13" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_createSPList_listName_Desc</v>
+        <v>66</v>
+      </c>
+      <c r="G13" s="2" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_createSPList_addContentType_name_Desc</v>
       </c>
       <c r="H13" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Schema_createSPList_listName_Desc:"The name of the List",</v>
+        <v>Schema_createSPList_addContentType_name_Desc:"The name of an existing Site Content Type",</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_createSPList_templateType_Title</v>
+        <v>65</v>
+      </c>
+      <c r="D14" s="2" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_createSPList_removeContentType_name_Title</v>
       </c>
       <c r="E14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Schema_createSPList_templateType_Title:"List's Template Type",</v>
+        <v>Schema_createSPList_removeContentType_name_Title:"Content Type's name",</v>
       </c>
       <c r="F14" t="s">
-        <v>81</v>
-      </c>
-      <c r="G14" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_createSPList_templateType_Desc</v>
+        <v>67</v>
+      </c>
+      <c r="G14" s="2" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_createSPList_removeContentType_name_Desc</v>
       </c>
       <c r="H14" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Schema_createSPList_templateType_Desc:"The template type of the list",</v>
+        <v>Schema_createSPList_removeContentType_name_Desc:"The name of the Content Type",</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D15" t="str">
         <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_createSPList_subactions_Title</v>
+        <v>Schema_createSPList_setSPFieldCustomFormatter_fieldDisplayName_Title</v>
       </c>
       <c r="E15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Schema_createSPList_subactions_Title:"Sub actions",</v>
+        <v>Schema_createSPList_setSPFieldCustomFormatter_fieldDisplayName_Title:"Field's display name",</v>
       </c>
       <c r="F15" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="G15" t="str">
         <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_createSPList_subactions_Desc</v>
+        <v>Schema_createSPList_setSPFieldCustomFormatter_fieldDisplayName_Desc</v>
       </c>
       <c r="H15" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Schema_createSPList_subactions_Desc:"Define the sub actions of the Create List action",</v>
+        <v>Schema_createSPList_setSPFieldCustomFormatter_fieldDisplayName_Desc:"The display name of the field to apply the formatting on",</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D16" s="2" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_addNavLink_url_Title</v>
-      </c>
-      <c r="E16" s="6" t="str">
-        <f>D16&amp;":"""&amp;C16&amp;""","</f>
-        <v>Schema_addNavLink_url_Title:"Link's URL",</v>
+        <v>71</v>
+      </c>
+      <c r="D16" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_createSPList_setSPFieldCustomFormatter_formatterJSON_Title</v>
+      </c>
+      <c r="E16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Schema_createSPList_setSPFieldCustomFormatter_formatterJSON_Title:"The formatter JSON",</v>
       </c>
       <c r="F16" t="s">
-        <v>87</v>
-      </c>
-      <c r="G16" s="2" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_addNavLink_url_Desc</v>
-      </c>
-      <c r="H16" s="6" t="str">
-        <f>G16&amp;":"""&amp;F16&amp;""","</f>
-        <v>Schema_addNavLink_url_Desc:"The URL of the navigation Link",</v>
+        <v>73</v>
+      </c>
+      <c r="G16" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_createSPList_setSPFieldCustomFormatter_formatterJSON_Desc</v>
+      </c>
+      <c r="H16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Schema_createSPList_setSPFieldCustomFormatter_formatterJSON_Desc:"The formatter rules expressed in JSON",</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
-        <v>89</v>
-      </c>
-      <c r="D17" s="2" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_addNavLink_displayName_Title</v>
-      </c>
-      <c r="E17" s="6" t="str">
-        <f>D17&amp;":"""&amp;C17&amp;""","</f>
-        <v>Schema_addNavLink_displayName_Title:"Link's text",</v>
+        <v>77</v>
+      </c>
+      <c r="D17" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_createSPList_listName_Title</v>
+      </c>
+      <c r="E17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Schema_createSPList_listName_Title:"List's name",</v>
       </c>
       <c r="F17" t="s">
-        <v>86</v>
-      </c>
-      <c r="G17" s="2" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_addNavLink_displayName_Desc</v>
-      </c>
-      <c r="H17" s="6" t="str">
-        <f>G17&amp;":"""&amp;F17&amp;""","</f>
-        <v>Schema_addNavLink_displayName_Desc:"The text of the navigation Link",</v>
+        <v>80</v>
+      </c>
+      <c r="G17" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_createSPList_listName_Desc</v>
+      </c>
+      <c r="H17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Schema_createSPList_listName_Desc:"The name of the List",</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
-        <v>90</v>
-      </c>
-      <c r="D18" s="2" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_addNavLink_isWebRelative_Title</v>
-      </c>
-      <c r="E18" s="6" t="str">
-        <f>D18&amp;":"""&amp;C18&amp;""","</f>
-        <v>Schema_addNavLink_isWebRelative_Title:"Is Web Relative",</v>
+        <v>78</v>
+      </c>
+      <c r="D18" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_createSPList_templateType_Title</v>
+      </c>
+      <c r="E18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Schema_createSPList_templateType_Title:"List's Template Type",</v>
       </c>
       <c r="F18" t="s">
-        <v>85</v>
-      </c>
-      <c r="G18" s="2" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_addNavLink_isWebRelative_Desc</v>
-      </c>
-      <c r="H18" s="6" t="str">
-        <f>G18&amp;":"""&amp;F18&amp;""","</f>
-        <v>Schema_addNavLink_isWebRelative_Desc:"Is the URL of the link web-relative ?",</v>
+        <v>81</v>
+      </c>
+      <c r="G18" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_createSPList_templateType_Desc</v>
+      </c>
+      <c r="H18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Schema_createSPList_templateType_Desc:"The template type of the list",</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" s="2" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_applyTheme_themeName_Title</v>
-      </c>
-      <c r="E19" s="6" t="str">
-        <f>D19&amp;":"""&amp;C19&amp;""","</f>
-        <v>Schema_applyTheme_themeName_Title:"Theme's name",</v>
+        <v>79</v>
+      </c>
+      <c r="D19" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_createSPList_subactions_Title</v>
+      </c>
+      <c r="E19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Schema_createSPList_subactions_Title:"Sub actions",</v>
       </c>
       <c r="F19" t="s">
-        <v>93</v>
-      </c>
-      <c r="G19" s="2" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_applyTheme_themeName_Desc</v>
-      </c>
-      <c r="H19" s="6" t="str">
-        <f>G19&amp;":"""&amp;F19&amp;""","</f>
-        <v>Schema_applyTheme_themeName_Desc:"The name of the custom theme to apply",</v>
+        <v>82</v>
+      </c>
+      <c r="G19" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_createSPList_subactions_Desc</v>
+      </c>
+      <c r="H19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Schema_createSPList_subactions_Desc:"Define the sub actions of the Create List action",</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
         <v>83</v>
       </c>
       <c r="C20" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D20" s="2" t="str">
         <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_setSiteLogo_url_Title</v>
+        <v>Schema_addNavLink_url_Title</v>
       </c>
       <c r="E20" s="6" t="str">
         <f>D20&amp;":"""&amp;C20&amp;""","</f>
-        <v>Schema_setSiteLogo_url_Title:"Site logo's URL",</v>
+        <v>Schema_addNavLink_url_Title:"Link's URL",</v>
       </c>
       <c r="F20" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="G20" s="2" t="str">
         <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_setSiteLogo_url_Desc</v>
+        <v>Schema_addNavLink_url_Desc</v>
       </c>
       <c r="H20" s="6" t="str">
         <f>G20&amp;":"""&amp;F20&amp;""","</f>
-        <v>Schema_setSiteLogo_url_Desc:"The URL of the Site logo",</v>
+        <v>Schema_addNavLink_url_Desc:"The URL of the navigation Link",</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>96</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_joinHubSite_hubSiteId_Title</v>
-      </c>
-      <c r="E21" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Schema_joinHubSite_hubSiteId_Title:"Hub Site",</v>
+        <v>89</v>
+      </c>
+      <c r="D21" s="2" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_addNavLink_displayName_Title</v>
+      </c>
+      <c r="E21" s="6" t="str">
+        <f>D21&amp;":"""&amp;C21&amp;""","</f>
+        <v>Schema_addNavLink_displayName_Title:"Link's text",</v>
       </c>
       <c r="F21" t="s">
-        <v>98</v>
-      </c>
-      <c r="G21" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_joinHubSite_hubSiteId_Desc</v>
-      </c>
-      <c r="H21" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Schema_joinHubSite_hubSiteId_Desc:"The identifier of the Hub Site",</v>
+        <v>86</v>
+      </c>
+      <c r="G21" s="2" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_addNavLink_displayName_Desc</v>
+      </c>
+      <c r="H21" s="6" t="str">
+        <f>G21&amp;":"""&amp;F21&amp;""","</f>
+        <v>Schema_addNavLink_displayName_Desc:"The text of the navigation Link",</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D22" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_triggerFlow_url_Title</v>
-      </c>
-      <c r="E22" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Schema_triggerFlow_url_Title:"Flow's URL",</v>
+        <v>90</v>
+      </c>
+      <c r="D22" s="2" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_addNavLink_isWebRelative_Title</v>
+      </c>
+      <c r="E22" s="6" t="str">
+        <f>D22&amp;":"""&amp;C22&amp;""","</f>
+        <v>Schema_addNavLink_isWebRelative_Title:"Is Web Relative",</v>
       </c>
       <c r="F22" t="s">
-        <v>105</v>
-      </c>
-      <c r="G22" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_triggerFlow_url_Desc</v>
-      </c>
-      <c r="H22" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Schema_triggerFlow_url_Desc:"The URL of the Flow to trigger",</v>
+        <v>85</v>
+      </c>
+      <c r="G22" s="2" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_addNavLink_isWebRelative_Desc</v>
+      </c>
+      <c r="H22" s="6" t="str">
+        <f>G22&amp;":"""&amp;F22&amp;""","</f>
+        <v>Schema_addNavLink_isWebRelative_Desc:"Is the URL of the link web-relative ?",</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
-      </c>
-      <c r="D23" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_triggerFlow_name_Title</v>
-      </c>
-      <c r="E23" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Schema_triggerFlow_name_Title:"Flow's name",</v>
+        <v>92</v>
+      </c>
+      <c r="D23" s="2" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_applyTheme_themeName_Title</v>
+      </c>
+      <c r="E23" s="6" t="str">
+        <f>D23&amp;":"""&amp;C23&amp;""","</f>
+        <v>Schema_applyTheme_themeName_Title:"Theme's name",</v>
       </c>
       <c r="F23" t="s">
-        <v>104</v>
-      </c>
-      <c r="G23" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_triggerFlow_name_Desc</v>
-      </c>
-      <c r="H23" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Schema_triggerFlow_name_Desc:"The name of the Flow to trigger",</v>
+        <v>93</v>
+      </c>
+      <c r="G23" s="2" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_applyTheme_themeName_Desc</v>
+      </c>
+      <c r="H23" s="6" t="str">
+        <f>G23&amp;":"""&amp;F23&amp;""","</f>
+        <v>Schema_applyTheme_themeName_Desc:"The name of the custom theme to apply",</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>102</v>
-      </c>
-      <c r="D24" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_triggerFlow_parameters_Title</v>
-      </c>
-      <c r="E24" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Schema_triggerFlow_parameters_Title:"Flow's parameters",</v>
+        <v>94</v>
+      </c>
+      <c r="D24" s="2" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_setSiteLogo_url_Title</v>
+      </c>
+      <c r="E24" s="6" t="str">
+        <f>D24&amp;":"""&amp;C24&amp;""","</f>
+        <v>Schema_setSiteLogo_url_Title:"Site logo's URL",</v>
       </c>
       <c r="F24" t="s">
-        <v>103</v>
-      </c>
-      <c r="G24" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
-        <v>Schema_triggerFlow_parameters_Desc</v>
-      </c>
-      <c r="H24" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Schema_triggerFlow_parameters_Desc:"The set of parameters of the Flow",</v>
+        <v>95</v>
+      </c>
+      <c r="G24" s="2" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_setSiteLogo_url_Desc</v>
+      </c>
+      <c r="H24" s="6" t="str">
+        <f>G24&amp;":"""&amp;F24&amp;""","</f>
+        <v>Schema_setSiteLogo_url_Desc:"The URL of the Site logo",</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_joinHubSite_hubSiteId_Title</v>
+      </c>
+      <c r="E25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Schema_joinHubSite_hubSiteId_Title:"Hub Site",</v>
+      </c>
+      <c r="F25" t="s">
+        <v>98</v>
+      </c>
+      <c r="G25" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_joinHubSite_hubSiteId_Desc</v>
+      </c>
+      <c r="H25" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Schema_joinHubSite_hubSiteId_Desc:"The identifier of the Hub Site",</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_triggerFlow_url_Title</v>
+      </c>
+      <c r="E26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Schema_triggerFlow_url_Title:"Flow's URL",</v>
+      </c>
+      <c r="F26" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_triggerFlow_url_Desc</v>
+      </c>
+      <c r="H26" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Schema_triggerFlow_url_Desc:"The URL of the Flow to trigger",</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_triggerFlow_name_Title</v>
+      </c>
+      <c r="E27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Schema_triggerFlow_name_Title:"Flow's name",</v>
+      </c>
+      <c r="F27" t="s">
+        <v>104</v>
+      </c>
+      <c r="G27" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_triggerFlow_name_Desc</v>
+      </c>
+      <c r="H27" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Schema_triggerFlow_name_Desc:"The name of the Flow to trigger",</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_triggerFlow_parameters_Title</v>
+      </c>
+      <c r="E28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Schema_triggerFlow_parameters_Title:"Flow's parameters",</v>
+      </c>
+      <c r="F28" t="s">
+        <v>103</v>
+      </c>
+      <c r="G28" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
+        <v>Schema_triggerFlow_parameters_Desc</v>
+      </c>
+      <c r="H28" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Schema_triggerFlow_parameters_Desc:"The set of parameters of the Flow",</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
         <v>106</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B29" t="s">
         <v>109</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C29" t="s">
         <v>110</v>
       </c>
-      <c r="D25" t="str">
+      <c r="D29" t="str">
         <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Title","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
         <v>Schema_setSiteExternalSharingCapability_capability_Title</v>
       </c>
-      <c r="E25" s="1" t="str">
+      <c r="E29" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Schema_setSiteExternalSharingCapability_capability_Title:"External sharing capability",</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F29" t="s">
         <v>111</v>
       </c>
-      <c r="G25" t="str">
+      <c r="G29" t="str">
         <f>SUBSTITUTE(SUBSTITUTE("Schema_${actionId}_${value}_Desc","${value}",Table13[[#This Row],[Property]]),"${actionId}",Table13[[#This Row],[Action]])</f>
         <v>Schema_setSiteExternalSharingCapability_capability_Desc</v>
       </c>
-      <c r="H25" s="1" t="str">
+      <c r="H29" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Schema_setSiteExternalSharingCapability_capability_Desc:"The defined external sharing capability",</v>
       </c>

</xml_diff>